<commit_message>
Confirgured multiple table generation
</commit_message>
<xml_diff>
--- a/Daily-Sales.xlsx
+++ b/Daily-Sales.xlsx
@@ -113,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -124,83 +124,83 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>44468.85239583333</v>
-      </c>
-      <c r="D4" t="n">
-        <v>873.0</v>
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>44468.85549768519</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>44468.85239583333</v>
       </c>
       <c r="D5" t="n">
-        <v>7348.0</v>
+        <v>873.0</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>44468.85549768519</v>
+      </c>
+      <c r="D6" t="n">
+        <v>7348.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C7" s="3" t="n">
         <v>44469.06122685185</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>2093.0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto Column sizing Added
</commit_message>
<xml_diff>
--- a/Daily-Sales.xlsx
+++ b/Daily-Sales.xlsx
@@ -118,6 +118,14 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.60546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="21.13671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.39453125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.2890625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.57421875" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>